<commit_message>
new layout and week07
</commit_message>
<xml_diff>
--- a/2023/week07/data.xlsx
+++ b/2023/week07/data.xlsx
@@ -41,9 +41,6 @@
     <t xml:space="preserve">Programas básicos </t>
   </si>
   <si>
-    <t>enrolments</t>
-  </si>
-  <si>
     <t>local</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>Agriculture, forestry and fishing</t>
+  </si>
+  <si>
+    <t>enrollments</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +496,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -505,7 +505,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -513,13 +513,13 @@
         <v>2020</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
@@ -533,16 +533,16 @@
         <v>2020</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" s="1">
         <v>234594</v>
@@ -553,16 +553,16 @@
         <v>2020</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="1">
         <v>67415</v>
@@ -573,16 +573,16 @@
         <v>2020</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="1">
         <v>209623</v>
@@ -593,16 +593,16 @@
         <v>2020</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="1">
         <v>671393</v>
@@ -613,16 +613,16 @@
         <v>2020</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1">
         <v>54480</v>
@@ -633,16 +633,16 @@
         <v>2020</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="1">
         <v>113573</v>
@@ -653,16 +653,16 @@
         <v>2020</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9" s="1">
         <v>401756</v>
@@ -673,16 +673,16 @@
         <v>2020</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" s="1">
         <v>131639</v>
@@ -693,16 +693,16 @@
         <v>2020</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="1">
         <v>568803</v>
@@ -713,16 +713,16 @@
         <v>2020</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F12" s="1">
         <v>37797</v>
@@ -733,13 +733,13 @@
         <v>2020</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>4</v>
@@ -753,16 +753,16 @@
         <v>2020</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" s="1">
         <v>324625</v>
@@ -773,16 +773,16 @@
         <v>2020</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" s="1">
         <v>41838</v>
@@ -793,16 +793,16 @@
         <v>2020</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" s="1">
         <v>142406</v>
@@ -813,16 +813,16 @@
         <v>2020</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" s="1">
         <v>548354</v>
@@ -833,16 +833,16 @@
         <v>2020</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F18" s="1">
         <v>43687</v>
@@ -853,16 +853,16 @@
         <v>2020</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F19" s="1">
         <v>81690</v>
@@ -873,16 +873,16 @@
         <v>2020</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20" s="1">
         <v>282122</v>
@@ -893,16 +893,16 @@
         <v>2020</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F21" s="1">
         <v>92027</v>
@@ -913,16 +913,16 @@
         <v>2020</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F22" s="1">
         <v>476042</v>
@@ -933,16 +933,16 @@
         <v>2020</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F23" s="1">
         <v>33872</v>
@@ -953,13 +953,13 @@
         <v>2020</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>4</v>
@@ -973,16 +973,16 @@
         <v>2020</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" s="1">
         <v>370700</v>
@@ -993,16 +993,16 @@
         <v>2020</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26" s="1">
         <v>28079</v>
@@ -1013,16 +1013,16 @@
         <v>2020</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F27" s="1">
         <v>14042</v>
@@ -1033,16 +1033,16 @@
         <v>2020</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" s="1">
         <v>448144</v>
@@ -1053,16 +1053,16 @@
         <v>2020</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F29" s="1">
         <v>3850</v>
@@ -1073,16 +1073,16 @@
         <v>2020</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F30" s="1">
         <v>71030</v>
@@ -1093,16 +1093,16 @@
         <v>2020</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F31" s="1">
         <v>64503</v>
@@ -1113,16 +1113,16 @@
         <v>2020</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F32" s="1">
         <v>8812</v>
@@ -1133,16 +1133,16 @@
         <v>2020</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F33" s="1">
         <v>124976</v>
@@ -1153,16 +1153,16 @@
         <v>2020</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F34" s="1">
         <v>45828</v>
@@ -1173,13 +1173,13 @@
         <v>2020</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>4</v>
@@ -1193,16 +1193,16 @@
         <v>2020</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F36" s="1">
         <v>394686</v>
@@ -1213,16 +1213,16 @@
         <v>2020</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" s="1">
         <v>20175</v>
@@ -1233,16 +1233,16 @@
         <v>2020</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" s="1">
         <v>10154</v>
@@ -1253,16 +1253,16 @@
         <v>2020</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" s="1">
         <v>411670</v>
@@ -1273,16 +1273,16 @@
         <v>2020</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F40" s="1">
         <v>2870</v>
@@ -1293,16 +1293,16 @@
         <v>2020</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F41" s="1">
         <v>55124</v>
@@ -1313,16 +1313,16 @@
         <v>2020</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F42" s="1">
         <v>53051</v>
@@ -1333,16 +1333,16 @@
         <v>2020</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F43" s="1">
         <v>6837</v>
@@ -1353,16 +1353,16 @@
         <v>2020</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F44" s="1">
         <v>189290</v>
@@ -1373,16 +1373,16 @@
         <v>2020</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F45" s="1">
         <v>47878</v>

</xml_diff>